<commit_message>
Add "normal" formatting to template
Enrich the Excel template with some normal formatting as well. Also, add 
two more sheets with conditional formatting and one sheet without 
(Codebook). This will allow us to test how Stata's export excel affects 
other Excel sheets.
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -8,12 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Finn Woelm\Projects\stata-excel-template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2525CD7-2AF0-422C-A901-BE61CE11CF1F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EB5012C-F422-47FD-A1F2-115B5BC57D0F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="825" yWindow="-120" windowWidth="28095" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2505" yWindow="1560" windowWidth="25140" windowHeight="11835" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Overall Results" sheetId="8" r:id="rId1"/>
+    <sheet name="Values, Ratings, Trends" sheetId="2" r:id="rId2"/>
+    <sheet name="Values, Scores, Ratings, Trends" sheetId="9" r:id="rId3"/>
+    <sheet name="Codebook" sheetId="7" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,12 +28,48 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="14">
   <si>
     <t>title</t>
   </si>
   <si>
     <t>conditional formatting for the entire sheet (A:ZZ)</t>
+  </si>
+  <si>
+    <t>green</t>
+  </si>
+  <si>
+    <t>yellow</t>
+  </si>
+  <si>
+    <t>orange</t>
+  </si>
+  <si>
+    <t>red</t>
+  </si>
+  <si>
+    <t>gray</t>
+  </si>
+  <si>
+    <t>↑</t>
+  </si>
+  <si>
+    <t>↓</t>
+  </si>
+  <si>
+    <t>➚</t>
+  </si>
+  <si>
+    <t>→</t>
+  </si>
+  <si>
+    <t>hello</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>value</t>
   </si>
 </sst>
 </file>
@@ -80,19 +119,244 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="45"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment textRotation="45"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{98D6A88B-4311-433F-94EE-C83666F9F6A6}"/>
   </cellStyles>
-  <dxfs count="18">
+  <dxfs count="27">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <u/>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <u/>
+        <color theme="7" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <u/>
+        <color rgb="FFEA6B14"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <u/>
+        <color rgb="FFC00000"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -810,12 +1074,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:D6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CAFD747-961D-4958-B282-966AFB409A3E}">
+  <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -834,16 +1097,79 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D6" s="3"/>
-    </row>
+    <row r="3" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="3">
+        <v>15.5</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="3">
+        <v>27.6</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="4"/>
+    </row>
+    <row r="7" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="17" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="18" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="19" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="20" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <conditionalFormatting sqref="A1:ZZ1048576">
+  <conditionalFormatting sqref="A1:ZZ1048576 AAA1:XFD1">
     <cfRule type="containsText" dxfId="17" priority="1" operator="containsText" text="↓">
       <formula>NOT(ISERROR(SEARCH("↓",A1)))</formula>
     </cfRule>
@@ -875,4 +1201,308 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3AF4C6E-3E65-4E26-AFB9-A800448A3220}">
+  <dimension ref="A1:D20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="9.140625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" s="1" customFormat="1" ht="27" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="3">
+        <v>15.5</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="3">
+        <v>27.6</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="4"/>
+    </row>
+    <row r="7" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="17" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="18" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="19" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="20" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <conditionalFormatting sqref="A1:ZZ1048576 AAA1:XFD1">
+    <cfRule type="containsText" dxfId="26" priority="1" operator="containsText" text="↓">
+      <formula>NOT(ISERROR(SEARCH("↓",A1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="25" priority="2" operator="containsText" text="→">
+      <formula>NOT(ISERROR(SEARCH("→",A1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="24" priority="3" operator="containsText" text="➚">
+      <formula>NOT(ISERROR(SEARCH("➚",A1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="23" priority="4" operator="containsText" text="↑">
+      <formula>NOT(ISERROR(SEARCH("↑",A1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="22" priority="5" operator="containsText" text="gray">
+      <formula>NOT(ISERROR(SEARCH("gray",A1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="21" priority="6" operator="containsText" text="orange">
+      <formula>NOT(ISERROR(SEARCH("orange",A1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="20" priority="7" operator="containsText" text="yellow">
+      <formula>NOT(ISERROR(SEARCH("yellow",A1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="19" priority="8" operator="containsText" text="red">
+      <formula>NOT(ISERROR(SEARCH("red",A1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="18" priority="9" operator="containsText" text="green">
+      <formula>NOT(ISERROR(SEARCH("green",A1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81D59EDA-29EF-4B54-BF6D-02E731E6D405}">
+  <dimension ref="A1:D20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="9.140625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" s="1" customFormat="1" ht="27" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="3">
+        <v>15.5</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="3">
+        <v>27.6</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="4"/>
+    </row>
+    <row r="7" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="17" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="18" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="19" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="20" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <conditionalFormatting sqref="A1:ZZ1048576 AAA1:XFD1">
+    <cfRule type="containsText" dxfId="8" priority="1" operator="containsText" text="↓">
+      <formula>NOT(ISERROR(SEARCH("↓",A1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="7" priority="2" operator="containsText" text="→">
+      <formula>NOT(ISERROR(SEARCH("→",A1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="6" priority="3" operator="containsText" text="➚">
+      <formula>NOT(ISERROR(SEARCH("➚",A1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text="↑">
+      <formula>NOT(ISERROR(SEARCH("↑",A1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="gray">
+      <formula>NOT(ISERROR(SEARCH("gray",A1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="3" priority="6" operator="containsText" text="orange">
+      <formula>NOT(ISERROR(SEARCH("orange",A1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="2" priority="7" operator="containsText" text="yellow">
+      <formula>NOT(ISERROR(SEARCH("yellow",A1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="1" priority="8" operator="containsText" text="red">
+      <formula>NOT(ISERROR(SEARCH("red",A1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="0" priority="9" operator="containsText" text="green">
+      <formula>NOT(ISERROR(SEARCH("green",A1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4629F5CE-B5DB-4909-BAA5-331D2B62803D}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E5" sqref="E5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" s="5" customFormat="1" ht="27" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Template: Set last-opened sheet to "Overall results"
Excel stores what sheet was last opened and then opens that by default. 
We want the "Overall results" sheet to be the default tab.
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Finn Woelm\Projects\stata-excel-template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EB5012C-F422-47FD-A1F2-115B5BC57D0F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{108A10F6-77F2-440D-A377-96D51BAE0FD2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2505" yWindow="1560" windowWidth="25140" windowHeight="11835" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2505" yWindow="1560" windowWidth="25140" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overall Results" sheetId="8" r:id="rId1"/>
@@ -1077,7 +1077,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CAFD747-961D-4958-B282-966AFB409A3E}">
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
@@ -1170,31 +1170,31 @@
     <row r="20" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <conditionalFormatting sqref="A1:ZZ1048576 AAA1:XFD1">
-    <cfRule type="containsText" dxfId="17" priority="1" operator="containsText" text="↓">
+    <cfRule type="containsText" dxfId="26" priority="1" operator="containsText" text="↓">
       <formula>NOT(ISERROR(SEARCH("↓",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="16" priority="2" operator="containsText" text="→">
+    <cfRule type="containsText" dxfId="25" priority="2" operator="containsText" text="→">
       <formula>NOT(ISERROR(SEARCH("→",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="15" priority="3" operator="containsText" text="➚">
+    <cfRule type="containsText" dxfId="24" priority="3" operator="containsText" text="➚">
       <formula>NOT(ISERROR(SEARCH("➚",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="14" priority="4" operator="containsText" text="↑">
+    <cfRule type="containsText" dxfId="23" priority="4" operator="containsText" text="↑">
       <formula>NOT(ISERROR(SEARCH("↑",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="5" operator="containsText" text="gray">
+    <cfRule type="containsText" dxfId="22" priority="5" operator="containsText" text="gray">
       <formula>NOT(ISERROR(SEARCH("gray",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="6" operator="containsText" text="orange">
+    <cfRule type="containsText" dxfId="21" priority="6" operator="containsText" text="orange">
       <formula>NOT(ISERROR(SEARCH("orange",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="11" priority="7" operator="containsText" text="yellow">
+    <cfRule type="containsText" dxfId="20" priority="7" operator="containsText" text="yellow">
       <formula>NOT(ISERROR(SEARCH("yellow",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="8" operator="containsText" text="red">
+    <cfRule type="containsText" dxfId="19" priority="8" operator="containsText" text="red">
       <formula>NOT(ISERROR(SEARCH("red",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="9" priority="9" operator="containsText" text="green">
+    <cfRule type="containsText" dxfId="18" priority="9" operator="containsText" text="green">
       <formula>NOT(ISERROR(SEARCH("green",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1300,31 +1300,31 @@
     <row r="20" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <conditionalFormatting sqref="A1:ZZ1048576 AAA1:XFD1">
-    <cfRule type="containsText" dxfId="26" priority="1" operator="containsText" text="↓">
+    <cfRule type="containsText" dxfId="17" priority="1" operator="containsText" text="↓">
       <formula>NOT(ISERROR(SEARCH("↓",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="25" priority="2" operator="containsText" text="→">
+    <cfRule type="containsText" dxfId="16" priority="2" operator="containsText" text="→">
       <formula>NOT(ISERROR(SEARCH("→",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="24" priority="3" operator="containsText" text="➚">
+    <cfRule type="containsText" dxfId="15" priority="3" operator="containsText" text="➚">
       <formula>NOT(ISERROR(SEARCH("➚",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="23" priority="4" operator="containsText" text="↑">
+    <cfRule type="containsText" dxfId="14" priority="4" operator="containsText" text="↑">
       <formula>NOT(ISERROR(SEARCH("↑",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="22" priority="5" operator="containsText" text="gray">
+    <cfRule type="containsText" dxfId="13" priority="5" operator="containsText" text="gray">
       <formula>NOT(ISERROR(SEARCH("gray",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="21" priority="6" operator="containsText" text="orange">
+    <cfRule type="containsText" dxfId="12" priority="6" operator="containsText" text="orange">
       <formula>NOT(ISERROR(SEARCH("orange",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="20" priority="7" operator="containsText" text="yellow">
+    <cfRule type="containsText" dxfId="11" priority="7" operator="containsText" text="yellow">
       <formula>NOT(ISERROR(SEARCH("yellow",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="19" priority="8" operator="containsText" text="red">
+    <cfRule type="containsText" dxfId="10" priority="8" operator="containsText" text="red">
       <formula>NOT(ISERROR(SEARCH("red",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="18" priority="9" operator="containsText" text="green">
+    <cfRule type="containsText" dxfId="9" priority="9" operator="containsText" text="green">
       <formula>NOT(ISERROR(SEARCH("green",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1467,7 +1467,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4629F5CE-B5DB-4909-BAA5-331D2B62803D}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E5" sqref="E5"/>
     </sheetView>

</xml_diff>

<commit_message>
Template: Format headers with conditional formatting
Use conditional formatting to format header row (bold). Unfortunately,
the conditional formatting options do not include angled/slanted text.
So this strategy does not work. We will need to use Stata's put excel
command instead.
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Finn Woelm\Projects\stata-excel-template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{108A10F6-77F2-440D-A377-96D51BAE0FD2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0C6B9D0-E910-491C-92AA-CC4ADA4050E2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2505" yWindow="1560" windowWidth="25140" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="945" yWindow="1410" windowWidth="23040" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overall Results" sheetId="8" r:id="rId1"/>
@@ -76,16 +76,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -117,17 +109,17 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment textRotation="45"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="45"/>
     </xf>
   </cellXfs>
@@ -135,7 +127,14 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{98D6A88B-4311-433F-94EE-C83666F9F6A6}"/>
   </cellStyles>
-  <dxfs count="27">
+  <dxfs count="48">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -577,6 +576,462 @@
         <vertical/>
         <horizontal/>
       </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <u/>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <u/>
+        <color theme="7" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <u/>
+        <color rgb="FFEA6B14"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <u/>
+        <color rgb="FFC00000"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <u/>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <u/>
+        <color theme="7" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <u/>
+        <color rgb="FFEA6B14"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <u/>
+        <color rgb="FFC00000"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
     </dxf>
     <dxf>
       <fill>
@@ -1077,125 +1532,128 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CAFD747-961D-4958-B282-966AFB409A3E}">
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" ht="27" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:4" s="5" customFormat="1" ht="27" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="5" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+    <row r="3" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="2">
         <v>15.5</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+    <row r="4" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="2">
         <v>27.6</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+    <row r="5" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+    <row r="6" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="4"/>
-    </row>
-    <row r="7" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+      <c r="D6" s="3"/>
+    </row>
+    <row r="7" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="17" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="18" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="19" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="20" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="17" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="18" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="19" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="20" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <conditionalFormatting sqref="A1:ZZ1048576 AAA1:XFD1">
-    <cfRule type="containsText" dxfId="26" priority="1" operator="containsText" text="↓">
+    <cfRule type="containsText" dxfId="47" priority="2" operator="containsText" text="↓">
       <formula>NOT(ISERROR(SEARCH("↓",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="25" priority="2" operator="containsText" text="→">
+    <cfRule type="containsText" dxfId="46" priority="3" operator="containsText" text="→">
       <formula>NOT(ISERROR(SEARCH("→",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="24" priority="3" operator="containsText" text="➚">
+    <cfRule type="containsText" dxfId="45" priority="4" operator="containsText" text="➚">
       <formula>NOT(ISERROR(SEARCH("➚",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="23" priority="4" operator="containsText" text="↑">
+    <cfRule type="containsText" dxfId="44" priority="5" operator="containsText" text="↑">
       <formula>NOT(ISERROR(SEARCH("↑",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="22" priority="5" operator="containsText" text="gray">
+    <cfRule type="containsText" dxfId="43" priority="6" operator="containsText" text="gray">
       <formula>NOT(ISERROR(SEARCH("gray",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="21" priority="6" operator="containsText" text="orange">
+    <cfRule type="containsText" dxfId="42" priority="7" operator="containsText" text="orange">
       <formula>NOT(ISERROR(SEARCH("orange",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="20" priority="7" operator="containsText" text="yellow">
+    <cfRule type="containsText" dxfId="41" priority="8" operator="containsText" text="yellow">
       <formula>NOT(ISERROR(SEARCH("yellow",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="19" priority="8" operator="containsText" text="red">
+    <cfRule type="containsText" dxfId="40" priority="9" operator="containsText" text="red">
       <formula>NOT(ISERROR(SEARCH("red",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="18" priority="9" operator="containsText" text="green">
+    <cfRule type="containsText" dxfId="39" priority="10" operator="containsText" text="green">
       <formula>NOT(ISERROR(SEARCH("green",A1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1:XFD1">
+    <cfRule type="expression" dxfId="38" priority="1">
+      <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1205,127 +1663,145 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3AF4C6E-3E65-4E26-AFB9-A800448A3220}">
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" ht="27" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:3" s="5" customFormat="1" ht="27" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="5" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="2">
         <v>15.5</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="2">
         <v>27.6</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="4"/>
-    </row>
-    <row r="7" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="17" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="18" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="19" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="20" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <conditionalFormatting sqref="A1:ZZ1048576 AAA1:XFD1">
-    <cfRule type="containsText" dxfId="17" priority="1" operator="containsText" text="↓">
+  <conditionalFormatting sqref="A2:XFD1048576">
+    <cfRule type="containsText" dxfId="37" priority="11" operator="containsText" text="↓">
+      <formula>NOT(ISERROR(SEARCH("↓",A2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="36" priority="12" operator="containsText" text="→">
+      <formula>NOT(ISERROR(SEARCH("→",A2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="35" priority="13" operator="containsText" text="➚">
+      <formula>NOT(ISERROR(SEARCH("➚",A2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="34" priority="14" operator="containsText" text="↑">
+      <formula>NOT(ISERROR(SEARCH("↑",A2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="33" priority="15" operator="containsText" text="gray">
+      <formula>NOT(ISERROR(SEARCH("gray",A2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="32" priority="16" operator="containsText" text="orange">
+      <formula>NOT(ISERROR(SEARCH("orange",A2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="31" priority="17" operator="containsText" text="yellow">
+      <formula>NOT(ISERROR(SEARCH("yellow",A2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="30" priority="18" operator="containsText" text="red">
+      <formula>NOT(ISERROR(SEARCH("red",A2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="29" priority="19" operator="containsText" text="green">
+      <formula>NOT(ISERROR(SEARCH("green",A2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1:XFD1">
+    <cfRule type="containsText" dxfId="28" priority="2" operator="containsText" text="↓">
       <formula>NOT(ISERROR(SEARCH("↓",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="16" priority="2" operator="containsText" text="→">
+    <cfRule type="containsText" dxfId="27" priority="3" operator="containsText" text="→">
       <formula>NOT(ISERROR(SEARCH("→",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="15" priority="3" operator="containsText" text="➚">
+    <cfRule type="containsText" dxfId="26" priority="4" operator="containsText" text="➚">
       <formula>NOT(ISERROR(SEARCH("➚",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="14" priority="4" operator="containsText" text="↑">
+    <cfRule type="containsText" dxfId="25" priority="5" operator="containsText" text="↑">
       <formula>NOT(ISERROR(SEARCH("↑",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="5" operator="containsText" text="gray">
+    <cfRule type="containsText" dxfId="24" priority="6" operator="containsText" text="gray">
       <formula>NOT(ISERROR(SEARCH("gray",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="6" operator="containsText" text="orange">
+    <cfRule type="containsText" dxfId="23" priority="7" operator="containsText" text="orange">
       <formula>NOT(ISERROR(SEARCH("orange",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="11" priority="7" operator="containsText" text="yellow">
+    <cfRule type="containsText" dxfId="22" priority="8" operator="containsText" text="yellow">
       <formula>NOT(ISERROR(SEARCH("yellow",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="8" operator="containsText" text="red">
+    <cfRule type="containsText" dxfId="21" priority="9" operator="containsText" text="red">
       <formula>NOT(ISERROR(SEARCH("red",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="9" priority="9" operator="containsText" text="green">
+    <cfRule type="containsText" dxfId="20" priority="10" operator="containsText" text="green">
       <formula>NOT(ISERROR(SEARCH("green",A1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1:XFD1">
+    <cfRule type="expression" dxfId="19" priority="1">
+      <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1338,124 +1814,158 @@
   <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" ht="27" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:4" s="5" customFormat="1" ht="27" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="5" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+    <row r="3" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="2">
         <v>15.5</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+    <row r="4" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="2">
         <v>27.6</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+    <row r="5" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+    <row r="6" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="4"/>
-    </row>
-    <row r="7" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+      <c r="D6" s="3"/>
+    </row>
+    <row r="7" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="17" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="18" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="19" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="20" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="17" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="18" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="19" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="20" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <conditionalFormatting sqref="A1:ZZ1048576 AAA1:XFD1">
-    <cfRule type="containsText" dxfId="8" priority="1" operator="containsText" text="↓">
+  <conditionalFormatting sqref="A2:ZZ1048576">
+    <cfRule type="containsText" dxfId="18" priority="11" operator="containsText" text="↓">
+      <formula>NOT(ISERROR(SEARCH("↓",A2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="17" priority="12" operator="containsText" text="→">
+      <formula>NOT(ISERROR(SEARCH("→",A2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="16" priority="13" operator="containsText" text="➚">
+      <formula>NOT(ISERROR(SEARCH("➚",A2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="15" priority="14" operator="containsText" text="↑">
+      <formula>NOT(ISERROR(SEARCH("↑",A2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="14" priority="15" operator="containsText" text="gray">
+      <formula>NOT(ISERROR(SEARCH("gray",A2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="13" priority="16" operator="containsText" text="orange">
+      <formula>NOT(ISERROR(SEARCH("orange",A2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="12" priority="17" operator="containsText" text="yellow">
+      <formula>NOT(ISERROR(SEARCH("yellow",A2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="11" priority="18" operator="containsText" text="red">
+      <formula>NOT(ISERROR(SEARCH("red",A2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="10" priority="19" operator="containsText" text="green">
+      <formula>NOT(ISERROR(SEARCH("green",A2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1:XFD1">
+    <cfRule type="containsText" dxfId="9" priority="2" operator="containsText" text="↓">
       <formula>NOT(ISERROR(SEARCH("↓",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="2" operator="containsText" text="→">
+    <cfRule type="containsText" dxfId="8" priority="3" operator="containsText" text="→">
       <formula>NOT(ISERROR(SEARCH("→",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="3" operator="containsText" text="➚">
+    <cfRule type="containsText" dxfId="7" priority="4" operator="containsText" text="➚">
       <formula>NOT(ISERROR(SEARCH("➚",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text="↑">
+    <cfRule type="containsText" dxfId="6" priority="5" operator="containsText" text="↑">
       <formula>NOT(ISERROR(SEARCH("↑",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="gray">
+    <cfRule type="containsText" dxfId="5" priority="6" operator="containsText" text="gray">
       <formula>NOT(ISERROR(SEARCH("gray",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="6" operator="containsText" text="orange">
+    <cfRule type="containsText" dxfId="4" priority="7" operator="containsText" text="orange">
       <formula>NOT(ISERROR(SEARCH("orange",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="7" operator="containsText" text="yellow">
+    <cfRule type="containsText" dxfId="3" priority="8" operator="containsText" text="yellow">
       <formula>NOT(ISERROR(SEARCH("yellow",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="8" operator="containsText" text="red">
+    <cfRule type="containsText" dxfId="2" priority="9" operator="containsText" text="red">
       <formula>NOT(ISERROR(SEARCH("red",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="9" operator="containsText" text="green">
+    <cfRule type="containsText" dxfId="1" priority="10" operator="containsText" text="green">
       <formula>NOT(ISERROR(SEARCH("green",A1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1:XFD1">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1474,17 +1984,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" s="5" customFormat="1" ht="27" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:4" s="4" customFormat="1" ht="27" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="4" t="s">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Template: Change column widths
Test that Stata's excel export does not overwrite column widths. It does 
not :)
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Finn Woelm\Projects\stata-excel-template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FB2072B-F8E2-409C-8D0F-A5FF66218538}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{541A406C-E18C-4D33-AF88-2DABD1417005}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="945" yWindow="1410" windowWidth="23040" windowHeight="11835" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="945" yWindow="1410" windowWidth="23040" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overall Results" sheetId="8" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="17">
   <si>
     <t>title</t>
   </si>
@@ -71,6 +71,15 @@
   <si>
     <t>value</t>
   </si>
+  <si>
+    <t>big column</t>
+  </si>
+  <si>
+    <t>normal col</t>
+  </si>
+  <si>
+    <t>tiny</t>
+  </si>
 </sst>
 </file>
 
@@ -111,7 +120,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -121,6 +130,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="45" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1532,27 +1544,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CAFD747-961D-4958-B282-966AFB409A3E}">
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomRight" activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="32.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="4.42578125" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="5" customFormat="1" ht="27" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="5" customFormat="1" ht="48.75" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>0</v>
+        <v>14</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>16</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>0</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1823,7 +1837,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81D59EDA-29EF-4B54-BF6D-02E731E6D405}">
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>

</xml_diff>